<commit_message>
changed excels to text format
</commit_message>
<xml_diff>
--- a/RIF_OPTIMIZER_v1.xlsx
+++ b/RIF_OPTIMIZER_v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patdj\Documents\RIF\GUI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benka\Documents\GitHub\REBAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2797E4CF-EDC0-4552-8043-67D1B39160D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF9AE91-5D09-40F2-9AC0-B32D2AE1BDC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="64">
   <si>
     <t>Number</t>
   </si>
@@ -179,22 +179,6 @@
   </si>
   <si>
     <t xml:space="preserve">If a ticker has a flat weight, it is no longer part of a group. </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">File Format: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>RIF_PORT.csv</t>
-    </r>
   </si>
   <si>
     <t>FDN</t>
@@ -235,6 +219,28 @@
   </si>
   <si>
     <t xml:space="preserve">You cannot have a flat weight and a group at the same time. </t>
+  </si>
+  <si>
+    <t>1/1/2019</t>
+  </si>
+  <si>
+    <t>1/1/2016</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">File Name: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RIF_PORT.csv</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -751,9 +757,8 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -1119,121 +1124,121 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:9" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A8" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1250,237 +1255,240 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D12" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="6"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="M2" s="6">
+        <v>2</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E2">
+      <c r="E3" s="6">
         <v>0.2</v>
       </c>
-      <c r="F2">
+      <c r="F3" s="6">
         <v>0.4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2">
-        <v>0.01</v>
-      </c>
-      <c r="L2">
-        <v>0.25</v>
-      </c>
-      <c r="M2">
-        <v>2</v>
-      </c>
-      <c r="N2" t="s">
-        <v>18</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="R3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="S2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3">
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="6">
         <v>0.2</v>
       </c>
-      <c r="F3">
+      <c r="F7" s="6">
         <v>0.4</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="R3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4">
-        <v>0.2</v>
-      </c>
-      <c r="F4">
-        <v>0.4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="R4" t="s">
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5">
-        <v>0.2</v>
-      </c>
-      <c r="F5">
-        <v>0.4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6">
-        <v>0.2</v>
-      </c>
-      <c r="F6">
-        <v>0.4</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7">
-        <v>0.2</v>
-      </c>
-      <c r="F7">
-        <v>0.4</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8">
-        <v>0.02</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="G8" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1506,296 +1514,299 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="6"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="6">
         <v>0.15</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="6">
         <v>0.3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1">
-        <v>42370</v>
-      </c>
-      <c r="I2" s="1">
-        <v>43618</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="H2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="6">
         <v>0.05</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="6">
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <v>0.3</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="6">
         <v>0.45</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="6">
         <v>0.2</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="6">
         <v>0.4</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="6">
         <v>0.15</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="6">
         <v>0.3</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
         <v>0.3</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="6">
         <v>0.45</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>0.1</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>0.15</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="6">
         <v>0.3</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="6">
         <v>0.15</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="6">
         <v>0.3</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="6">
         <v>0.2</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="6">
         <v>0.4</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <v>0.2</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="6">
         <v>0.4</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>0.01</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>0.01</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1821,84 +1832,85 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="6"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="R2" t="s">
+      <c r="R2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="R3" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="R4" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R4" s="6" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>